<commit_message>
class digram file added
</commit_message>
<xml_diff>
--- a/المزايا الموجودة في ملف المشروع.xlsx
+++ b/المزايا الموجودة في ملف المشروع.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MegaFiles\Graduation Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0D9A5AF-66AF-42A0-8745-5896F47E6C7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1CFC045-938F-4B2A-868B-F35E39B7DF10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="مقارنة الثلاث فقرات" sheetId="1" r:id="rId1"/>
-    <sheet name="UseCases" sheetId="5" r:id="rId2"/>
-    <sheet name="MSCO" sheetId="3" r:id="rId3"/>
-    <sheet name="F-NF " sheetId="2" r:id="rId4"/>
-    <sheet name="الخلاصة " sheetId="4" r:id="rId5"/>
+    <sheet name="time table" sheetId="6" r:id="rId2"/>
+    <sheet name="UseCases" sheetId="5" r:id="rId3"/>
+    <sheet name="MSCO" sheetId="3" r:id="rId4"/>
+    <sheet name="F-NF " sheetId="2" r:id="rId5"/>
+    <sheet name="الخلاصة " sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="247">
   <si>
     <t>النقاط المستخرجة من فقرة "جملة المشكلة":</t>
   </si>
@@ -835,6 +836,45 @@
   </si>
   <si>
     <t>المستخدم ستصل بمستخدم آخر من خلال التطبيق</t>
+  </si>
+  <si>
+    <t>ch1</t>
+  </si>
+  <si>
+    <t>ch2</t>
+  </si>
+  <si>
+    <t>1-2023</t>
+  </si>
+  <si>
+    <t>12-2022</t>
+  </si>
+  <si>
+    <t>2-2023</t>
+  </si>
+  <si>
+    <t>3-2023</t>
+  </si>
+  <si>
+    <t>4-2023</t>
+  </si>
+  <si>
+    <t>5-2023</t>
+  </si>
+  <si>
+    <t>6-2023</t>
+  </si>
+  <si>
+    <t>breack</t>
+  </si>
+  <si>
+    <t>ch3</t>
+  </si>
+  <si>
+    <t>implemintaion</t>
+  </si>
+  <si>
+    <t>Testing</t>
   </si>
 </sst>
 </file>
@@ -944,7 +984,7 @@
       <charset val="178"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -991,6 +1031,24 @@
       <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1164,7 +1222,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1291,6 +1349,42 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="2"/>
     </xf>
@@ -1309,113 +1403,30 @@
     <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="عادي" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="16">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="178"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="178"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -1562,6 +1573,65 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="14"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="178"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="178"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
         <color auto="1"/>
         <name val="Arial"/>
         <family val="2"/>
@@ -1656,26 +1726,26 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B7F83B40-CD8E-4375-B587-F6BF963B81F7}" name="الجدول14" displayName="الجدول14" ref="A1:B99" totalsRowShown="0" headerRowDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B7F83B40-CD8E-4375-B587-F6BF963B81F7}" name="الجدول14" displayName="الجدول14" ref="A1:B99" totalsRowShown="0" headerRowDxfId="11">
   <autoFilter ref="A1:B99" xr:uid="{B7F83B40-CD8E-4375-B587-F6BF963B81F7}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{63DAEEFF-9488-42D3-8BE5-3719915B4702}" name="النقاط المستخرجة من فقرة &quot;جملة المشكلة&quot;:" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{75422B75-5C9F-4375-B1A5-4E9552D6E90D}" name="Use Cases" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{63DAEEFF-9488-42D3-8BE5-3719915B4702}" name="النقاط المستخرجة من فقرة &quot;جملة المشكلة&quot;:" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{75422B75-5C9F-4375-B1A5-4E9552D6E90D}" name="Use Cases" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{62EC1967-044F-4FF9-B07A-D86A6C181FE4}" name="الجدول2" displayName="الجدول2" ref="A1:F33" totalsRowShown="0" dataDxfId="10" headerRowBorderDxfId="11" tableBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{62EC1967-044F-4FF9-B07A-D86A6C181FE4}" name="الجدول2" displayName="الجدول2" ref="A1:F33" totalsRowShown="0" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6">
   <autoFilter ref="A1:F33" xr:uid="{62EC1967-044F-4FF9-B07A-D86A6C181FE4}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{31E7BB5E-302C-4455-9799-B34840BDAC81}" name="أساسي" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{96ACB727-7EE1-462C-A634-5F2FE86D0F34}" name="النوع" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{437E81CD-DD85-4609-8BFA-892D670DEBED}" name="MSCW" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{7D8FC975-A0FF-42AA-AD73-39923ED86BF7}" name="عمود1" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{52853365-F33D-4874-85E6-0DF1513E60B8}" name="Incriment No." dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{E62EC6BB-E9E9-411C-B1EC-F7E04A85F2DF}" name="عمود2" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{31E7BB5E-302C-4455-9799-B34840BDAC81}" name="أساسي" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{96ACB727-7EE1-462C-A634-5F2FE86D0F34}" name="النوع" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{437E81CD-DD85-4609-8BFA-892D670DEBED}" name="MSCW" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{7D8FC975-A0FF-42AA-AD73-39923ED86BF7}" name="عمود1" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{52853365-F33D-4874-85E6-0DF1513E60B8}" name="Incriment No." dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{E62EC6BB-E9E9-411C-B1EC-F7E04A85F2DF}" name="عمود2" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1947,7 +2017,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F1" sqref="A1:F24"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2199,11 +2269,151 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB655B24-27C5-4956-A781-57DA9BF58010}">
+  <dimension ref="A1:G10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.69921875" customWidth="1"/>
+    <col min="2" max="2" width="13.8984375" customWidth="1"/>
+    <col min="6" max="6" width="11.796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.59765625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="67" t="s">
+        <v>237</v>
+      </c>
+      <c r="B1" s="67" t="s">
+        <v>236</v>
+      </c>
+      <c r="C1" s="67" t="s">
+        <v>238</v>
+      </c>
+      <c r="D1" s="67" t="s">
+        <v>239</v>
+      </c>
+      <c r="E1" s="67" t="s">
+        <v>240</v>
+      </c>
+      <c r="F1" s="67" t="s">
+        <v>241</v>
+      </c>
+      <c r="G1" s="67" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="68" t="s">
+        <v>234</v>
+      </c>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="66"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="39"/>
+      <c r="B4" s="68" t="s">
+        <v>235</v>
+      </c>
+      <c r="C4" s="68" t="s">
+        <v>243</v>
+      </c>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="39"/>
+      <c r="B5" s="66"/>
+      <c r="C5" s="66"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="39"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="39"/>
+      <c r="B6" s="39"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="65" t="s">
+        <v>244</v>
+      </c>
+      <c r="E6" s="65"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
+    </row>
+    <row r="7" spans="1:7" s="64" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="66"/>
+      <c r="B7" s="66"/>
+      <c r="C7" s="66"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="66"/>
+      <c r="F7" s="66"/>
+      <c r="G7" s="66"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="39"/>
+      <c r="B8" s="39"/>
+      <c r="C8" s="39"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="69" t="s">
+        <v>245</v>
+      </c>
+      <c r="G8" s="39"/>
+    </row>
+    <row r="9" spans="1:7" s="64" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="66"/>
+      <c r="B9" s="66"/>
+      <c r="C9" s="66"/>
+      <c r="D9" s="66"/>
+      <c r="E9" s="66"/>
+      <c r="F9" s="66"/>
+      <c r="G9" s="66"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="39"/>
+      <c r="B10" s="39"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="70" t="s">
+        <v>246</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D6:E6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEE67B8C-D36A-4A5F-B792-E90BD931BB67}">
   <dimension ref="A1:C131"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A108" workbookViewId="0">
-      <selection activeCell="B126" sqref="B126"/>
+    <sheetView rightToLeft="1" topLeftCell="A117" workbookViewId="0">
+      <selection activeCell="A141" sqref="A141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2226,85 +2436,85 @@
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="59" t="s">
+      <c r="B2" s="52" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
-      <c r="B3" s="59" t="s">
+      <c r="B3" s="52" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
-      <c r="B4" s="59"/>
+      <c r="B4" s="52"/>
     </row>
     <row r="5" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="59" t="s">
+      <c r="B5" s="52" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
-      <c r="B6" s="59" t="s">
+      <c r="B6" s="52" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
-      <c r="B7" s="59" t="s">
+      <c r="B7" s="52" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
-      <c r="B8" s="59" t="s">
+      <c r="B8" s="52" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
-      <c r="B9" s="59" t="s">
+      <c r="B9" s="52" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
-      <c r="B10" s="59" t="s">
+      <c r="B10" s="52" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
-      <c r="B11" s="59" t="s">
+      <c r="B11" s="52" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
-      <c r="B12" s="59" t="s">
+      <c r="B12" s="52" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
-      <c r="B13" s="59" t="s">
+      <c r="B13" s="52" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
-      <c r="B14" s="59" t="s">
+      <c r="B14" s="52" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
-      <c r="B15" s="59" t="s">
+      <c r="B15" s="52" t="s">
         <v>161</v>
       </c>
     </row>
@@ -2312,53 +2522,53 @@
       <c r="A16" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="60"/>
+      <c r="B16" s="52"/>
     </row>
     <row r="17" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="59"/>
+      <c r="B17" s="52"/>
     </row>
     <row r="18" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
-      <c r="B18" s="59" t="s">
+      <c r="B18" s="52" t="s">
         <v>162</v>
       </c>
-      <c r="C18" s="62" t="s">
+      <c r="C18" s="57" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
-      <c r="B19" s="59" t="s">
+      <c r="B19" s="52" t="s">
         <v>163</v>
       </c>
-      <c r="C19" s="62"/>
+      <c r="C19" s="57"/>
     </row>
     <row r="20" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
-      <c r="B20" s="59" t="s">
+      <c r="B20" s="52" t="s">
         <v>164</v>
       </c>
-      <c r="C20" s="62"/>
+      <c r="C20" s="57"/>
     </row>
     <row r="21" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
-      <c r="B21" s="59" t="s">
+      <c r="B21" s="52" t="s">
         <v>165</v>
       </c>
-      <c r="C21" s="62"/>
+      <c r="C21" s="57"/>
     </row>
     <row r="22" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
-      <c r="B22" s="59"/>
+      <c r="B22" s="52"/>
     </row>
     <row r="23" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="59" t="s">
+      <c r="B23" s="52" t="s">
         <v>167</v>
       </c>
     </row>
@@ -2366,7 +2576,7 @@
       <c r="A24" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B24" s="59" t="s">
+      <c r="B24" s="52" t="s">
         <v>167</v>
       </c>
     </row>
@@ -2374,23 +2584,23 @@
       <c r="A25" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B25" s="59"/>
+      <c r="B25" s="52"/>
     </row>
     <row r="26" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A26" s="7"/>
-      <c r="B26" s="59" t="s">
+      <c r="B26" s="52" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
-      <c r="B27" s="59" t="s">
+      <c r="B27" s="52" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
-      <c r="B28" s="59" t="s">
+      <c r="B28" s="52" t="s">
         <v>170</v>
       </c>
     </row>
@@ -2398,7 +2608,7 @@
       <c r="A29" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B29" s="59" t="s">
+      <c r="B29" s="52" t="s">
         <v>167</v>
       </c>
     </row>
@@ -2406,17 +2616,17 @@
       <c r="A30" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="59"/>
+      <c r="B30" s="52"/>
     </row>
     <row r="31" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
-      <c r="B31" s="59" t="s">
+      <c r="B31" s="52" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
-      <c r="B32" s="59" t="s">
+      <c r="B32" s="52" t="s">
         <v>173</v>
       </c>
       <c r="C32" t="s">
@@ -2425,7 +2635,7 @@
     </row>
     <row r="33" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
-      <c r="B33" s="59" t="s">
+      <c r="B33" s="52" t="s">
         <v>174</v>
       </c>
     </row>
@@ -2433,7 +2643,7 @@
       <c r="A34" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B34" s="59" t="s">
+      <c r="B34" s="52" t="s">
         <v>175</v>
       </c>
       <c r="C34" t="s">
@@ -2444,57 +2654,57 @@
       <c r="A35" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B35" s="59"/>
+      <c r="B35" s="52"/>
     </row>
     <row r="36" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
-      <c r="B36" s="59" t="s">
+      <c r="B36" s="52" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
-      <c r="B37" s="59" t="s">
+      <c r="B37" s="52" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
-      <c r="B38" s="59" t="s">
+      <c r="B38" s="52" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
-      <c r="B39" s="59"/>
+      <c r="B39" s="52"/>
     </row>
     <row r="40" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B40" s="59"/>
+      <c r="B40" s="52"/>
     </row>
     <row r="41" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
-      <c r="B41" s="59" t="s">
+      <c r="B41" s="52" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
-      <c r="B42" s="59" t="s">
+      <c r="B42" s="52" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A43" s="7"/>
-      <c r="B43" s="59" t="s">
+      <c r="B43" s="52" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A44" s="7"/>
-      <c r="B44" s="59" t="s">
+      <c r="B44" s="52" t="s">
         <v>180</v>
       </c>
     </row>
@@ -2502,23 +2712,23 @@
       <c r="A45" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B45" s="59"/>
+      <c r="B45" s="52"/>
     </row>
     <row r="46" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A46" s="7"/>
-      <c r="B46" s="59" t="s">
+      <c r="B46" s="52" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A47" s="7"/>
-      <c r="B47" s="59" t="s">
+      <c r="B47" s="52" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A48" s="7"/>
-      <c r="B48" s="59" t="s">
+      <c r="B48" s="52" t="s">
         <v>186</v>
       </c>
     </row>
@@ -2526,17 +2736,17 @@
       <c r="A49" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B49" s="59"/>
+      <c r="B49" s="52"/>
     </row>
     <row r="50" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A50" s="7"/>
-      <c r="B50" s="59" t="s">
+      <c r="B50" s="52" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A51" s="7"/>
-      <c r="B51" s="59" t="s">
+      <c r="B51" s="52" t="s">
         <v>188</v>
       </c>
     </row>
@@ -2544,11 +2754,11 @@
       <c r="A52" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B52" s="59"/>
+      <c r="B52" s="52"/>
     </row>
     <row r="53" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A53" s="7"/>
-      <c r="B53" s="59" t="s">
+      <c r="B53" s="52" t="s">
         <v>189</v>
       </c>
     </row>
@@ -2556,17 +2766,17 @@
       <c r="A54" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B54" s="59"/>
+      <c r="B54" s="52"/>
     </row>
     <row r="55" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A55" s="7"/>
-      <c r="B55" s="59" t="s">
+      <c r="B55" s="52" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A56" s="7"/>
-      <c r="B56" s="59" t="s">
+      <c r="B56" s="52" t="s">
         <v>190</v>
       </c>
     </row>
@@ -2574,11 +2784,11 @@
       <c r="A57" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B57" s="59"/>
+      <c r="B57" s="52"/>
     </row>
     <row r="58" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A58" s="7"/>
-      <c r="B58" s="59" t="s">
+      <c r="B58" s="52" t="s">
         <v>192</v>
       </c>
     </row>
@@ -2586,11 +2796,11 @@
       <c r="A59" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B59" s="59"/>
+      <c r="B59" s="52"/>
     </row>
     <row r="60" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A60" s="7"/>
-      <c r="B60" s="59" t="s">
+      <c r="B60" s="52" t="s">
         <v>193</v>
       </c>
     </row>
@@ -2598,99 +2808,99 @@
       <c r="A61" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B61" s="59"/>
+      <c r="B61" s="52"/>
     </row>
     <row r="62" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A62" s="7"/>
-      <c r="B62" s="59" t="s">
+      <c r="B62" s="52" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A63" s="7"/>
-      <c r="B63" s="59" t="s">
+      <c r="B63" s="52" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A64" s="7"/>
-      <c r="B64" s="59" t="s">
+      <c r="B64" s="52" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A65" s="7"/>
-      <c r="B65" s="59" t="s">
+      <c r="B65" s="52" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A66" s="7"/>
-      <c r="B66" s="59" t="s">
+      <c r="B66" s="52" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A67" s="7"/>
-      <c r="B67" s="59" t="s">
+      <c r="B67" s="52" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A68" s="7"/>
-      <c r="B68" s="59" t="s">
+      <c r="B68" s="52" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A69" s="7"/>
-      <c r="B69" s="59"/>
+      <c r="B69" s="52"/>
     </row>
     <row r="70" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B70" s="59"/>
+      <c r="B70" s="52"/>
     </row>
     <row r="71" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A71" s="7"/>
-      <c r="B71" s="59" t="s">
+      <c r="B71" s="52" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A72" s="7"/>
-      <c r="B72" s="59" t="s">
+      <c r="B72" s="52" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A73" s="7"/>
-      <c r="B73" s="59" t="s">
+      <c r="B73" s="52" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A74" s="7"/>
-      <c r="B74" s="59" t="s">
+      <c r="B74" s="52" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A75" s="7"/>
-      <c r="B75" s="59" t="s">
+      <c r="B75" s="52" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A76" s="7"/>
-      <c r="B76" s="59" t="s">
+      <c r="B76" s="52" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A77" s="7"/>
-      <c r="B77" s="59" t="s">
+      <c r="B77" s="52" t="s">
         <v>207</v>
       </c>
       <c r="C77" t="s">
@@ -2699,29 +2909,29 @@
     </row>
     <row r="78" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="A78" s="6"/>
-      <c r="B78" s="61"/>
+      <c r="B78" s="53"/>
     </row>
     <row r="79" spans="1:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="A79" s="58" t="s">
+      <c r="A79" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B79" s="61"/>
+      <c r="B79" s="53"/>
     </row>
     <row r="80" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B80" s="59"/>
+      <c r="B80" s="52"/>
     </row>
     <row r="81" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A81" s="52"/>
-      <c r="B81" s="59" t="s">
+      <c r="A81" s="7"/>
+      <c r="B81" s="52" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A82" s="52"/>
-      <c r="B82" s="59" t="s">
+      <c r="A82" s="7"/>
+      <c r="B82" s="52" t="s">
         <v>211</v>
       </c>
       <c r="C82" t="s">
@@ -2729,8 +2939,8 @@
       </c>
     </row>
     <row r="83" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A83" s="52"/>
-      <c r="B83" s="59" t="s">
+      <c r="A83" s="7"/>
+      <c r="B83" s="52" t="s">
         <v>210</v>
       </c>
     </row>
@@ -2738,7 +2948,7 @@
       <c r="A84" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B84" s="59" t="s">
+      <c r="B84" s="52" t="s">
         <v>213</v>
       </c>
     </row>
@@ -2746,7 +2956,7 @@
       <c r="A85" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B85" s="59" t="s">
+      <c r="B85" s="52" t="s">
         <v>167</v>
       </c>
     </row>
@@ -2754,47 +2964,47 @@
       <c r="A86" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B86" s="59"/>
+      <c r="B86" s="52"/>
     </row>
     <row r="87" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A87" s="7"/>
-      <c r="B87" s="59" t="s">
+      <c r="B87" s="52" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A88" s="7"/>
-      <c r="B88" s="59" t="s">
+      <c r="B88" s="52" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A89" s="7"/>
-      <c r="B89" s="59" t="s">
+      <c r="B89" s="52" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A90" s="7"/>
-      <c r="B90" s="59" t="s">
+      <c r="B90" s="52" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A91" s="7"/>
-      <c r="B91" s="59" t="s">
+      <c r="B91" s="52" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A92" s="7"/>
-      <c r="B92" s="59" t="s">
+      <c r="B92" s="52" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A93" s="7"/>
-      <c r="B93" s="59" t="s">
+      <c r="B93" s="52" t="s">
         <v>220</v>
       </c>
     </row>
@@ -2802,17 +3012,17 @@
       <c r="A94" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B94" s="59"/>
-    </row>
-    <row r="95" spans="1:3" s="63" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A95" s="52"/>
-      <c r="B95" s="60" t="s">
+      <c r="B94" s="52"/>
+    </row>
+    <row r="95" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="A95" s="7"/>
+      <c r="B95" s="52" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A96" s="4"/>
-      <c r="B96" s="59" t="s">
+      <c r="B96" s="52" t="s">
         <v>222</v>
       </c>
     </row>
@@ -2820,236 +3030,236 @@
       <c r="A97" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B97" s="59"/>
+      <c r="B97" s="52"/>
     </row>
     <row r="98" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A98" s="7"/>
-      <c r="B98" s="59" t="s">
+      <c r="B98" s="52" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A99" s="7"/>
-      <c r="B99" s="59" t="s">
+      <c r="B99" s="52" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A100" s="53" t="s">
+      <c r="A100" s="46" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A101" s="54" t="s">
+      <c r="A101" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="B101" s="64" t="s">
+      <c r="B101" s="54" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A102" s="55" t="s">
+      <c r="A102" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="B102" s="64" t="s">
+      <c r="B102" s="54" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A103" s="54" t="s">
+      <c r="A103" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="B103" s="64" t="s">
+      <c r="B103" s="54" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A104" s="54" t="s">
+      <c r="A104" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="B104" s="64" t="s">
+      <c r="B104" s="54" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A105" s="54" t="s">
+      <c r="A105" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="B105" s="64" t="s">
+      <c r="B105" s="54" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A106" s="54" t="s">
+      <c r="A106" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="B106" s="64" t="s">
+      <c r="B106" s="54" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A107" s="56" t="s">
+      <c r="A107" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="B107" s="64" t="s">
+      <c r="B107" s="54" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A108" s="54" t="s">
+      <c r="A108" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="B108" s="64" t="s">
+      <c r="B108" s="54" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A109" s="56" t="s">
+      <c r="A109" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="B109" s="64" t="s">
+      <c r="B109" s="54" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A110" s="54" t="s">
+      <c r="A110" s="47" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A111" s="54"/>
-      <c r="B111" s="64" t="s">
+      <c r="A111" s="47"/>
+      <c r="B111" s="54" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A112" s="54"/>
-      <c r="B112" s="64"/>
+      <c r="A112" s="47"/>
+      <c r="B112" s="54"/>
     </row>
     <row r="113" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A113" s="56" t="s">
+      <c r="A113" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="B113" s="64" t="s">
+      <c r="B113" s="54" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A114" s="56" t="s">
+      <c r="A114" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="B114" s="64" t="s">
+      <c r="B114" s="54" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A115" s="56" t="s">
+      <c r="A115" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="B115" s="64" t="s">
+      <c r="B115" s="54" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A116" s="56" t="s">
+      <c r="A116" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="B116" s="64" t="s">
+      <c r="B116" s="54" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A117" s="54" t="s">
+      <c r="A117" s="47" t="s">
         <v>39</v>
       </c>
-      <c r="B117" s="64" t="s">
+      <c r="B117" s="54" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A118" s="57" t="s">
+      <c r="A118" s="50" t="s">
         <v>41</v>
       </c>
-      <c r="B118" s="64" t="s">
+      <c r="B118" s="54" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A119" s="54" t="s">
+      <c r="A119" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="B119" s="64" t="s">
+      <c r="B119" s="54" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="120" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A120" s="56" t="s">
+      <c r="A120" s="49" t="s">
         <v>46</v>
       </c>
-      <c r="B120" s="64" t="s">
+      <c r="B120" s="54" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="121" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A121" s="54" t="s">
+      <c r="A121" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="B121" s="64"/>
+      <c r="B121" s="54"/>
     </row>
     <row r="122" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A122" s="54"/>
-      <c r="B122" s="64" t="s">
+      <c r="A122" s="47"/>
+      <c r="B122" s="54" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A123" s="54"/>
-      <c r="B123" s="64" t="s">
+      <c r="A123" s="47"/>
+      <c r="B123" s="54" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="124" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A124" s="56" t="s">
+      <c r="A124" s="49" t="s">
         <v>50</v>
       </c>
-      <c r="B124" s="64" t="s">
+      <c r="B124" s="54" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="125" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A125" s="54" t="s">
+      <c r="A125" s="47" t="s">
         <v>51</v>
       </c>
-      <c r="B125" s="64" t="s">
+      <c r="B125" s="54" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="126" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A126" s="54" t="s">
+      <c r="A126" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="B126" s="64" t="s">
+      <c r="B126" s="54" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="B127" s="64"/>
+      <c r="B127" s="54"/>
     </row>
     <row r="128" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="B128" s="64"/>
+      <c r="B128" s="54"/>
     </row>
     <row r="129" spans="2:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="B129" s="64" t="s">
+      <c r="B129" s="54" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="130" spans="2:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="B130" s="65" t="s">
+      <c r="B130" s="55" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="131" spans="2:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="B131" s="66" t="s">
+      <c r="B131" s="56" t="s">
         <v>55</v>
       </c>
     </row>
@@ -3064,7 +3274,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{927609CE-47BD-4AB6-8890-4D959C4F2FB9}">
   <dimension ref="A1:F43"/>
   <sheetViews>
@@ -3716,7 +3926,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7439FEE0-696D-4243-82B2-9DD996438AAB}">
   <dimension ref="A1:D61"/>
   <sheetViews>
@@ -3783,24 +3993,24 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A5" s="46"/>
-      <c r="B5" s="48" t="s">
+      <c r="A5" s="58"/>
+      <c r="B5" s="60" t="s">
         <v>64</v>
       </c>
       <c r="C5" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="D5" s="50" t="s">
+      <c r="D5" s="62" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="47"/>
-      <c r="B6" s="49"/>
+      <c r="A6" s="59"/>
+      <c r="B6" s="61"/>
       <c r="C6" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="D6" s="51"/>
+      <c r="D6" s="63"/>
     </row>
     <row r="7" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="25"/>
@@ -4078,24 +4288,24 @@
       </c>
     </row>
     <row r="38" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A38" s="46"/>
-      <c r="B38" s="48" t="s">
+      <c r="A38" s="58"/>
+      <c r="B38" s="60" t="s">
         <v>64</v>
       </c>
       <c r="C38" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="D38" s="50" t="s">
+      <c r="D38" s="62" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="47"/>
-      <c r="B39" s="49"/>
+      <c r="A39" s="59"/>
+      <c r="B39" s="61"/>
       <c r="C39" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="D39" s="51"/>
+      <c r="D39" s="63"/>
     </row>
     <row r="40" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="19"/>
@@ -4331,7 +4541,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BBE630F-5546-4F96-92B4-5C78DD28C667}">
   <dimension ref="A1:E28"/>
   <sheetViews>

</xml_diff>